<commit_message>
Input reading from csv completed
</commit_message>
<xml_diff>
--- a/Traffic.xlsx
+++ b/Traffic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\HPPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE36D6BC-169A-4DCD-A6D7-8A460972C63D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5278AA6D-43E7-4F30-BAF6-9DE6F21A0B07}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8790F61F-3959-4FDF-AF4E-C0DDF1FDC353}"/>
   </bookViews>
@@ -4799,7 +4799,7 @@
   <dimension ref="B1:AG16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="35.4" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>